<commit_message>
Change PO customer_code to supplier_code
</commit_message>
<xml_diff>
--- a/template/Po_Template.xlsx
+++ b/template/Po_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sky Ng\xampp\htdocs\synctronix\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2897D7-F092-4C02-8E19-2B352AE98E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D93175-1D70-4629-B9AD-F623D3C1B550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
   </bookViews>
@@ -28,12 +28,6 @@
     <t>Company Name</t>
   </si>
   <si>
-    <t>Customer Code</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
     <t>Site Code</t>
   </si>
   <si>
@@ -62,6 +56,12 @@
   </si>
   <si>
     <t>Delivery Date (DD-MM-YYYY)</t>
+  </si>
+  <si>
+    <t>Supplier Code</t>
+  </si>
+  <si>
+    <t>Supplier Name</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,40 +456,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed PO changed to Destination
</commit_message>
<xml_diff>
--- a/template/Po_Template.xlsx
+++ b/template/Po_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sky Ng\xampp\htdocs\synctronix\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihbi\xampp\htdocs\synctronix\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D93175-1D70-4629-B9AD-F623D3C1B550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D534319-68C8-4379-A36D-6CAEBF0F54CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
   </bookViews>
   <sheets>
     <sheet name="customermaster" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Company Code</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Salesrep Name</t>
   </si>
   <si>
-    <t>Deliver to Name</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -62,6 +59,12 @@
   </si>
   <si>
     <t>Supplier Name</t>
+  </si>
+  <si>
+    <t>Destination Code</t>
+  </si>
+  <si>
+    <t>Destination Name</t>
   </si>
 </sst>
 </file>
@@ -424,31 +427,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7AE52E-5E3F-4816-BCAD-C318F36103B6}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,10 +460,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -468,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -477,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>6</v>
@@ -486,10 +490,13 @@
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new fields in PO screen
</commit_message>
<xml_diff>
--- a/template/Po_Template.xlsx
+++ b/template/Po_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihbi\xampp\htdocs\synctronix\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D534319-68C8-4379-A36D-6CAEBF0F54CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCC21DF-2EBA-4005-A011-450D1F56FE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Company Code</t>
   </si>
@@ -65,6 +65,21 @@
   </si>
   <si>
     <t>Destination Name</t>
+  </si>
+  <si>
+    <t>Deliver To Name</t>
+  </si>
+  <si>
+    <t>Raw Material Code</t>
+  </si>
+  <si>
+    <t>Raw Material Name</t>
+  </si>
+  <si>
+    <t>Supplier Load</t>
+  </si>
+  <si>
+    <t>Supplier Quantity</t>
   </si>
 </sst>
 </file>
@@ -427,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7AE52E-5E3F-4816-BCAD-C318F36103B6}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,10 +464,15 @@
     <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,6 +516,21 @@
         <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial po screen push
</commit_message>
<xml_diff>
--- a/template/Po_Template.xlsx
+++ b/template/Po_Template.xlsx
@@ -5,39 +5,89 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihbi\xampp\htdocs\synctronix\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\EastRockNAS\EastRockAccount\E - Blacktop Lanchang Sdn Bhd\PWS\Test Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2509B033-9A5B-4276-9A0E-A34154BFBED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5145E19-6C83-492C-8B2C-4EF7AB52CAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F3DAB60-5F41-469D-B0E6-DE3C072237FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="customermaster" sheetId="1" r:id="rId1"/>
+    <sheet name="Super Extra special Import" sheetId="17" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>DocDate</t>
-  </si>
-  <si>
-    <t>DocNo</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>CompanyName</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+  <si>
+    <t>BN04</t>
+  </si>
+  <si>
+    <t>3/8WC</t>
+  </si>
+  <si>
+    <t>KUANTAN</t>
+  </si>
+  <si>
+    <t>PDR8379</t>
+  </si>
+  <si>
+    <t>WJY6528</t>
+  </si>
+  <si>
+    <t>CASH  SALES</t>
+  </si>
+  <si>
+    <t>501A-011</t>
+  </si>
+  <si>
+    <t>PREMIX WASTE</t>
+  </si>
+  <si>
+    <t>ADG3671</t>
+  </si>
+  <si>
+    <t>JERANTUT</t>
+  </si>
+  <si>
+    <t>S01730</t>
+  </si>
+  <si>
+    <t>MENTAKAB</t>
+  </si>
+  <si>
+    <t>S01772</t>
+  </si>
+  <si>
+    <t>BDM</t>
+  </si>
+  <si>
+    <t>GEB</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>MT</t>
   </si>
   <si>
     <t>PROJECT</t>
   </si>
   <si>
-    <t>ItemCode</t>
+    <t>LOCATION</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -46,38 +96,108 @@
     <t>DESCRIPTION2</t>
   </si>
   <si>
-    <t xml:space="preserve">  Qty  </t>
-  </si>
-  <si>
-    <t>UOM</t>
+    <t>REMARK2</t>
   </si>
   <si>
     <t>REMARK1</t>
   </si>
   <si>
-    <t>REMARK2</t>
+    <t>DOCNOEX</t>
+  </si>
+  <si>
+    <t>UNITPRICE</t>
+  </si>
+  <si>
+    <t>300-C0001</t>
+  </si>
+  <si>
+    <t>BL/SO2502/Test1</t>
+  </si>
+  <si>
+    <t>BL/SO2502/Test2</t>
+  </si>
+  <si>
+    <t>BL/SO2502/Test3</t>
+  </si>
+  <si>
+    <t>Testing 1</t>
+  </si>
+  <si>
+    <t>Testing 2</t>
+  </si>
+  <si>
+    <t>Testing 3</t>
+  </si>
+  <si>
+    <t>SHIPPER</t>
   </si>
   <si>
     <t>DOCREF1</t>
   </si>
   <si>
+    <t>CANCELLED</t>
+  </si>
+  <si>
+    <t>DOCNO</t>
+  </si>
+  <si>
+    <t>DOCDATE</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>COMPANYNAME</t>
+  </si>
+  <si>
+    <t>ITEMCODE</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>C0011</t>
+  </si>
+  <si>
+    <t>C0010</t>
+  </si>
+  <si>
+    <t>C0012</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>DOCREF2</t>
   </si>
   <si>
     <t>DOCREF3</t>
   </si>
   <si>
-    <t xml:space="preserve"> UNITPRICE </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amount </t>
+    <t>AGENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,23 +206,333 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -110,21 +540,249 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC00"/>
+      <color rgb="FFFF33CC"/>
+      <color rgb="FF9966FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -137,9 +795,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -177,7 +835,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -283,7 +941,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -425,101 +1083,288 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7AE52E-5E3F-4816-BCAD-C318F36103B6}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3CA383-87DB-4C9D-AB01-45416BEAC384}">
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>45737</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="7">
+        <v>5.39</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="10">
+        <v>23</v>
+      </c>
+      <c r="U2" s="10">
+        <v>123.97</v>
+      </c>
+      <c r="V2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>45737</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="7">
+        <v>3.55</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="10">
+        <v>23</v>
+      </c>
+      <c r="U3" s="10">
+        <v>81.649999999999991</v>
+      </c>
+      <c r="V3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>45737</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="7">
+        <v>2.95</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="S4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" s="10">
+        <v>260</v>
+      </c>
+      <c r="U4" s="10">
+        <v>767</v>
+      </c>
+      <c r="V4" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push for remarks pulling and auto population
</commit_message>
<xml_diff>
--- a/template/Po_Template.xlsx
+++ b/template/Po_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihbi\xampp\htdocs\synctronix\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\synctronix\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA02ADD-BAF8-418B-90B2-68CF47052110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F08AE1-CD23-4782-B11E-1CADAEA00203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F3DAB60-5F41-469D-B0E6-DE3C072237FB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>UOM</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>AGENT</t>
+  </si>
+  <si>
+    <t>DOCREF4</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -616,10 +619,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -983,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3CA383-87DB-4C9D-AB01-45416BEAC384}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,17 +1002,17 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1053,60 +1055,60 @@
       <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="8"/>
-      <c r="R2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="8"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="7"/>
+      <c r="T2" s="2"/>
       <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="8"/>
-      <c r="R3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="8"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="7"/>
+      <c r="T3" s="2"/>
       <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="8"/>
-      <c r="R4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="8"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="7"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="V4" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>